<commit_message>
Investment Policy Statement October 2021 update
</commit_message>
<xml_diff>
--- a/research/Asset Allocation Policy.xlsx
+++ b/research/Asset Allocation Policy.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fervidinc-my.sharepoint.com/personal/vitaly_kuznetsov_vitalik_net/Documents/Documents/Research/Investment Strategy/Reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fervidinc-my.sharepoint.com/personal/vitaly_kuznetsov_vitalik_net/Documents/Documents/Research/Investment Strategy/2021-10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{5ADBF5F3-7C6E-4C73-B3C0-5443D0E8D8B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8EF31E95-7854-4D80-B3F6-6B3BA966E67D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A06BFFD0-20B0-4DFF-B639-4173B08CCA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3600" windowWidth="29040" windowHeight="18240" xr2:uid="{85BB8F84-C9D2-4A53-8D40-3B5232B0A841}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{85BB8F84-C9D2-4A53-8D40-3B5232B0A841}"/>
   </bookViews>
   <sheets>
     <sheet name="Target Allocation" sheetId="1" r:id="rId1"/>
     <sheet name="Global Equities" sheetId="2" r:id="rId2"/>
-    <sheet name="Global FI and Alts ex. Reserve" sheetId="3" r:id="rId3"/>
-    <sheet name="Reserve" sheetId="4" r:id="rId4"/>
+    <sheet name="Global FI, Alts, and Reserve" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Global Equities</t>
   </si>
@@ -84,16 +83,10 @@
     <t>Global Equities Exposure</t>
   </si>
   <si>
-    <t>Reserve</t>
+    <t>Global Fixed Income,  Alternatives, and Reserve Exposure</t>
   </si>
   <si>
-    <t>Reserve Exposure</t>
-  </si>
-  <si>
-    <t>Global Fixed Income and Alternatives (ex Reserve)</t>
-  </si>
-  <si>
-    <t>Global Fixed Income and Alternatives (ex. Reserve) Exposure</t>
+    <t>Global Fixed Income, Alternatives, and Reserve</t>
   </si>
 </sst>
 </file>
@@ -146,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,12 +161,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,7 +188,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -268,19 +255,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -602,62 +580,54 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="22"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="C3" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>3</v>
       </c>
@@ -668,377 +638,276 @@
         <f>$B$4</f>
         <v>17</v>
       </c>
-      <c r="D4" s="23">
-        <f>$B$4</f>
-        <v>17</v>
-      </c>
-      <c r="E4" s="24"/>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>44561</v>
       </c>
       <c r="B6" s="5">
         <f>B$2-(B$2-B$3)/B$4*(YEAR($A6)-YEAR($A$6))</f>
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" ref="C6:D6" si="0">C$2-(C$2-C$3)/C$4*(YEAR($A6)-YEAR($A$6))</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C6" si="0">C$2-(C$2-C$3)/C$4*(YEAR($A6)-YEAR($A$6))</f>
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>44926</v>
       </c>
       <c r="B7" s="5">
-        <f t="shared" ref="B7:D23" si="1">B$2-(B$2-B$3)/B$4*(YEAR($A7)-YEAR($A$6))</f>
-        <v>0.68823529411764706</v>
+        <f t="shared" ref="B7:C23" si="1">B$2-(B$2-B$3)/B$4*(YEAR($A7)-YEAR($A$6))</f>
+        <v>0.88235294117647056</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>1.7647058823529412E-2</v>
-      </c>
-      <c r="D7" s="5">
-        <f t="shared" si="1"/>
-        <v>0.29411764705882354</v>
-      </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.11764705882352942</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45291</v>
       </c>
       <c r="B8" s="5">
         <f t="shared" si="1"/>
-        <v>0.67647058823529405</v>
+        <v>0.86470588235294121</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>3.5294117647058823E-2</v>
-      </c>
-      <c r="D8" s="5">
-        <f t="shared" si="1"/>
-        <v>0.28823529411764703</v>
-      </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.13529411764705884</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>45657</v>
       </c>
       <c r="B9" s="5">
         <f t="shared" si="1"/>
-        <v>0.66470588235294115</v>
+        <v>0.84705882352941175</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>5.2941176470588235E-2</v>
-      </c>
-      <c r="D9" s="5">
-        <f t="shared" si="1"/>
-        <v>0.28235294117647058</v>
-      </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.15294117647058825</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>46022</v>
       </c>
       <c r="B10" s="5">
         <f t="shared" si="1"/>
-        <v>0.65294117647058825</v>
+        <v>0.8294117647058824</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>7.0588235294117646E-2</v>
-      </c>
-      <c r="D10" s="5">
-        <f t="shared" si="1"/>
-        <v>0.27647058823529413</v>
-      </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.17058823529411765</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>46387</v>
       </c>
       <c r="B11" s="5">
         <f t="shared" si="1"/>
-        <v>0.64117647058823524</v>
+        <v>0.81176470588235294</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>8.8235294117647051E-2</v>
-      </c>
-      <c r="D11" s="5">
-        <f t="shared" si="1"/>
-        <v>0.27058823529411763</v>
-      </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.18823529411764708</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>46752</v>
       </c>
       <c r="B12" s="5">
         <f t="shared" si="1"/>
-        <v>0.62941176470588234</v>
+        <v>0.79411764705882359</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>0.10588235294117647</v>
-      </c>
-      <c r="D12" s="5">
-        <f t="shared" si="1"/>
-        <v>0.26470588235294118</v>
-      </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.20588235294117649</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>47118</v>
       </c>
       <c r="B13" s="5">
         <f t="shared" si="1"/>
-        <v>0.61764705882352944</v>
+        <v>0.77647058823529413</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>0.12352941176470589</v>
-      </c>
-      <c r="D13" s="5">
-        <f t="shared" si="1"/>
-        <v>0.25882352941176467</v>
-      </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.22352941176470592</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>47483</v>
       </c>
       <c r="B14" s="5">
         <f t="shared" si="1"/>
-        <v>0.60588235294117643</v>
+        <v>0.75882352941176467</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>0.14117647058823529</v>
-      </c>
-      <c r="D14" s="5">
-        <f t="shared" si="1"/>
-        <v>0.25294117647058822</v>
-      </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.24117647058823533</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>47848</v>
       </c>
       <c r="B15" s="5">
         <f t="shared" si="1"/>
-        <v>0.59411764705882353</v>
+        <v>0.74117647058823533</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>0.1588235294117647</v>
-      </c>
-      <c r="D15" s="5">
-        <f t="shared" si="1"/>
-        <v>0.24705882352941178</v>
-      </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.25882352941176473</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>48213</v>
       </c>
       <c r="B16" s="5">
         <f t="shared" si="1"/>
-        <v>0.58235294117647052</v>
+        <v>0.72352941176470587</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>0.1764705882352941</v>
-      </c>
-      <c r="D16" s="5">
-        <f t="shared" si="1"/>
-        <v>0.2411764705882353</v>
-      </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.27647058823529413</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>48579</v>
       </c>
       <c r="B17" s="5">
         <f t="shared" si="1"/>
-        <v>0.57058823529411762</v>
+        <v>0.70588235294117641</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>0.19411764705882353</v>
-      </c>
-      <c r="D17" s="5">
-        <f t="shared" si="1"/>
-        <v>0.23529411764705882</v>
-      </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.29411764705882359</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>48944</v>
       </c>
       <c r="B18" s="5">
         <f t="shared" si="1"/>
-        <v>0.55882352941176472</v>
+        <v>0.68823529411764706</v>
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>0.21176470588235294</v>
-      </c>
-      <c r="D18" s="5">
-        <f t="shared" si="1"/>
-        <v>0.22941176470588237</v>
-      </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.31176470588235294</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>49309</v>
       </c>
       <c r="B19" s="5">
         <f t="shared" si="1"/>
-        <v>0.54705882352941171</v>
+        <v>0.6705882352941176</v>
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>0.22941176470588234</v>
-      </c>
-      <c r="D19" s="5">
-        <f t="shared" si="1"/>
-        <v>0.22352941176470587</v>
-      </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.3294117647058824</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>49674</v>
       </c>
       <c r="B20" s="5">
         <f t="shared" si="1"/>
-        <v>0.53529411764705881</v>
+        <v>0.65294117647058825</v>
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>0.24705882352941178</v>
-      </c>
-      <c r="D20" s="5">
-        <f t="shared" si="1"/>
-        <v>0.21764705882352942</v>
-      </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.34705882352941181</v>
+      </c>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>50040</v>
       </c>
       <c r="B21" s="5">
         <f t="shared" si="1"/>
-        <v>0.5235294117647058</v>
+        <v>0.63529411764705879</v>
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>0.26470588235294118</v>
-      </c>
-      <c r="D21" s="5">
-        <f t="shared" si="1"/>
-        <v>0.21176470588235294</v>
-      </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.36470588235294121</v>
+      </c>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>50405</v>
       </c>
       <c r="B22" s="14">
         <f t="shared" si="1"/>
-        <v>0.5117647058823529</v>
+        <v>0.61764705882352944</v>
       </c>
       <c r="C22" s="14">
         <f t="shared" si="1"/>
-        <v>0.28235294117647058</v>
-      </c>
-      <c r="D22" s="14">
-        <f t="shared" si="1"/>
-        <v>0.20588235294117646</v>
-      </c>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.38235294117647067</v>
+      </c>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
         <v>50770</v>
       </c>
       <c r="B23" s="26">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="C23" s="26">
         <f t="shared" si="1"/>
-        <v>0.3</v>
-      </c>
-      <c r="D23" s="26">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="33" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="35" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="36" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="37" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="43" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="46" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="47" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="49" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="50" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="51" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="52" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="54" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" location="'Global Equities'!A1" display="Global Equities" xr:uid="{A9A8A7DD-8257-4E8C-B7BD-C9E5F3B82983}"/>
-    <hyperlink ref="C1" location="'Global FI and Alts ex. Reserve'!A1" display="Global Fixed Income and Alternatives (ex Reserve)" xr:uid="{8C7C0C6C-DECF-416D-8C26-35223B11C03D}"/>
-    <hyperlink ref="D1" location="Reserve!A1" display="Reserve" xr:uid="{A2DB1439-8CBB-47B5-853B-1DC81F8E2FCF}"/>
+    <hyperlink ref="C1" location="'Global FI, Alts, and Reserve'!A1" display="Global Fixed Income, Alternatives, and Reserve" xr:uid="{8C7C0C6C-DECF-416D-8C26-35223B11C03D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1072,7 +941,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="18">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -1122,25 +991,25 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34" t="s">
+      <c r="G5" s="32"/>
+      <c r="H5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="34"/>
+      <c r="I5" s="32"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="34"/>
+      <c r="L5" s="32"/>
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1185,40 +1054,40 @@
       </c>
       <c r="B7" s="14">
         <f>'Target Allocation'!B6</f>
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="C7" s="15">
         <f>B7*$B$2</f>
-        <v>0.52499999999999991</v>
+        <v>0.58500000000000008</v>
       </c>
       <c r="D7" s="15">
         <f>B7*$B$3</f>
-        <v>0.77</v>
+        <v>0.9900000000000001</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="14">
         <f>C7</f>
-        <v>0.52499999999999991</v>
+        <v>0.58500000000000008</v>
       </c>
       <c r="G7" s="14">
         <f>D7</f>
-        <v>0.77</v>
+        <v>0.9900000000000001</v>
       </c>
       <c r="H7" s="12">
         <v>0</v>
       </c>
       <c r="I7" s="15">
         <f>(G7-F7)*-1</f>
-        <v>-0.24500000000000011</v>
+        <v>-0.40500000000000003</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="14">
         <f>C7</f>
-        <v>0.52499999999999991</v>
+        <v>0.58500000000000008</v>
       </c>
       <c r="L7" s="14">
         <f>SUM(G7, ABS(I7))</f>
-        <v>1.0150000000000001</v>
+        <v>1.395</v>
       </c>
       <c r="M7" s="6"/>
     </row>
@@ -1229,40 +1098,40 @@
       </c>
       <c r="B8" s="14">
         <f>'Target Allocation'!B7</f>
-        <v>0.68823529411764706</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="C8" s="15">
         <f t="shared" ref="C8:C24" si="0">B8*$B$2</f>
-        <v>0.51617647058823524</v>
+        <v>0.57352941176470584</v>
       </c>
       <c r="D8" s="15">
         <f t="shared" ref="D8:D24" si="1">B8*$B$3</f>
-        <v>0.75705882352941178</v>
+        <v>0.97058823529411775</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="14">
         <f t="shared" ref="F8:F24" si="2">C8</f>
-        <v>0.51617647058823524</v>
+        <v>0.57352941176470584</v>
       </c>
       <c r="G8" s="14">
         <f t="shared" ref="G8:G24" si="3">D8</f>
-        <v>0.75705882352941178</v>
+        <v>0.97058823529411775</v>
       </c>
       <c r="H8" s="12">
         <v>0</v>
       </c>
       <c r="I8" s="15">
         <f t="shared" ref="I8:I24" si="4">(G8-F8)*-1</f>
-        <v>-0.24088235294117655</v>
+        <v>-0.39705882352941191</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="14">
         <f t="shared" ref="K8:K24" si="5">C8</f>
-        <v>0.51617647058823524</v>
+        <v>0.57352941176470584</v>
       </c>
       <c r="L8" s="14">
         <f t="shared" ref="L8:L24" si="6">SUM(G8, ABS(I8))</f>
-        <v>0.99794117647058833</v>
+        <v>1.3676470588235297</v>
       </c>
       <c r="M8" s="6"/>
     </row>
@@ -1273,40 +1142,40 @@
       </c>
       <c r="B9" s="14">
         <f>'Target Allocation'!B8</f>
-        <v>0.67647058823529405</v>
+        <v>0.86470588235294121</v>
       </c>
       <c r="C9" s="15">
         <f t="shared" si="0"/>
-        <v>0.50735294117647056</v>
+        <v>0.56205882352941183</v>
       </c>
       <c r="D9" s="15">
         <f t="shared" si="1"/>
-        <v>0.74411764705882355</v>
+        <v>0.9511764705882354</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="14">
         <f t="shared" si="2"/>
-        <v>0.50735294117647056</v>
+        <v>0.56205882352941183</v>
       </c>
       <c r="G9" s="14">
         <f t="shared" si="3"/>
-        <v>0.74411764705882355</v>
+        <v>0.9511764705882354</v>
       </c>
       <c r="H9" s="12">
         <v>0</v>
       </c>
       <c r="I9" s="15">
         <f t="shared" si="4"/>
-        <v>-0.23676470588235299</v>
+        <v>-0.38911764705882357</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="14">
         <f t="shared" si="5"/>
-        <v>0.50735294117647056</v>
+        <v>0.56205882352941183</v>
       </c>
       <c r="L9" s="14">
         <f t="shared" si="6"/>
-        <v>0.98088235294117654</v>
+        <v>1.3402941176470589</v>
       </c>
       <c r="M9" s="6"/>
     </row>
@@ -1317,40 +1186,40 @@
       </c>
       <c r="B10" s="14">
         <f>'Target Allocation'!B9</f>
-        <v>0.66470588235294115</v>
+        <v>0.84705882352941175</v>
       </c>
       <c r="C10" s="15">
         <f t="shared" si="0"/>
-        <v>0.49852941176470589</v>
+        <v>0.55058823529411771</v>
       </c>
       <c r="D10" s="15">
         <f t="shared" si="1"/>
-        <v>0.73117647058823532</v>
+        <v>0.93176470588235305</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="14">
         <f t="shared" si="2"/>
-        <v>0.49852941176470589</v>
+        <v>0.55058823529411771</v>
       </c>
       <c r="G10" s="14">
         <f t="shared" si="3"/>
-        <v>0.73117647058823532</v>
+        <v>0.93176470588235305</v>
       </c>
       <c r="H10" s="12">
         <v>0</v>
       </c>
       <c r="I10" s="15">
         <f t="shared" si="4"/>
-        <v>-0.23264705882352943</v>
+        <v>-0.38117647058823534</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="14">
         <f t="shared" si="5"/>
-        <v>0.49852941176470589</v>
+        <v>0.55058823529411771</v>
       </c>
       <c r="L10" s="14">
         <f t="shared" si="6"/>
-        <v>0.96382352941176475</v>
+        <v>1.3129411764705883</v>
       </c>
       <c r="M10" s="6"/>
     </row>
@@ -1361,40 +1230,40 @@
       </c>
       <c r="B11" s="14">
         <f>'Target Allocation'!B10</f>
-        <v>0.65294117647058825</v>
+        <v>0.8294117647058824</v>
       </c>
       <c r="C11" s="15">
         <f t="shared" si="0"/>
-        <v>0.48970588235294121</v>
+        <v>0.53911764705882359</v>
       </c>
       <c r="D11" s="15">
         <f t="shared" si="1"/>
-        <v>0.71823529411764708</v>
+        <v>0.9123529411764707</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="14">
         <f t="shared" si="2"/>
-        <v>0.48970588235294121</v>
+        <v>0.53911764705882359</v>
       </c>
       <c r="G11" s="14">
         <f t="shared" si="3"/>
-        <v>0.71823529411764708</v>
+        <v>0.9123529411764707</v>
       </c>
       <c r="H11" s="12">
         <v>0</v>
       </c>
       <c r="I11" s="15">
         <f t="shared" si="4"/>
-        <v>-0.22852941176470587</v>
+        <v>-0.37323529411764711</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="14">
         <f t="shared" si="5"/>
-        <v>0.48970588235294121</v>
+        <v>0.53911764705882359</v>
       </c>
       <c r="L11" s="14">
         <f t="shared" si="6"/>
-        <v>0.94676470588235295</v>
+        <v>1.2855882352941177</v>
       </c>
       <c r="M11" s="6"/>
     </row>
@@ -1405,40 +1274,40 @@
       </c>
       <c r="B12" s="14">
         <f>'Target Allocation'!B11</f>
-        <v>0.64117647058823524</v>
+        <v>0.81176470588235294</v>
       </c>
       <c r="C12" s="15">
         <f t="shared" si="0"/>
-        <v>0.48088235294117643</v>
+        <v>0.52764705882352947</v>
       </c>
       <c r="D12" s="15">
         <f t="shared" si="1"/>
-        <v>0.70529411764705885</v>
+        <v>0.89294117647058835</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="14">
         <f t="shared" si="2"/>
-        <v>0.48088235294117643</v>
+        <v>0.52764705882352947</v>
       </c>
       <c r="G12" s="14">
         <f t="shared" si="3"/>
-        <v>0.70529411764705885</v>
+        <v>0.89294117647058835</v>
       </c>
       <c r="H12" s="12">
         <v>0</v>
       </c>
       <c r="I12" s="15">
         <f t="shared" si="4"/>
-        <v>-0.22441176470588242</v>
+        <v>-0.36529411764705888</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="14">
         <f t="shared" si="5"/>
-        <v>0.48088235294117643</v>
+        <v>0.52764705882352947</v>
       </c>
       <c r="L12" s="14">
         <f t="shared" si="6"/>
-        <v>0.92970588235294127</v>
+        <v>1.2582352941176471</v>
       </c>
       <c r="M12" s="6"/>
     </row>
@@ -1449,40 +1318,40 @@
       </c>
       <c r="B13" s="14">
         <f>'Target Allocation'!B12</f>
-        <v>0.62941176470588234</v>
+        <v>0.79411764705882359</v>
       </c>
       <c r="C13" s="15">
         <f t="shared" si="0"/>
-        <v>0.47205882352941175</v>
+        <v>0.51617647058823535</v>
       </c>
       <c r="D13" s="15">
         <f t="shared" si="1"/>
-        <v>0.69235294117647062</v>
+        <v>0.873529411764706</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="14">
         <f t="shared" si="2"/>
-        <v>0.47205882352941175</v>
+        <v>0.51617647058823535</v>
       </c>
       <c r="G13" s="14">
         <f t="shared" si="3"/>
-        <v>0.69235294117647062</v>
+        <v>0.873529411764706</v>
       </c>
       <c r="H13" s="12">
         <v>0</v>
       </c>
       <c r="I13" s="15">
         <f t="shared" si="4"/>
-        <v>-0.22029411764705886</v>
+        <v>-0.35735294117647065</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="14">
         <f t="shared" si="5"/>
-        <v>0.47205882352941175</v>
+        <v>0.51617647058823535</v>
       </c>
       <c r="L13" s="14">
         <f t="shared" si="6"/>
-        <v>0.91264705882352948</v>
+        <v>1.2308823529411765</v>
       </c>
       <c r="M13" s="6"/>
     </row>
@@ -1493,40 +1362,40 @@
       </c>
       <c r="B14" s="14">
         <f>'Target Allocation'!B13</f>
-        <v>0.61764705882352944</v>
+        <v>0.77647058823529413</v>
       </c>
       <c r="C14" s="15">
         <f t="shared" si="0"/>
-        <v>0.46323529411764708</v>
+        <v>0.50470588235294123</v>
       </c>
       <c r="D14" s="15">
         <f t="shared" si="1"/>
-        <v>0.67941176470588238</v>
+        <v>0.85411764705882365</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="14">
         <f t="shared" si="2"/>
-        <v>0.46323529411764708</v>
+        <v>0.50470588235294123</v>
       </c>
       <c r="G14" s="14">
         <f t="shared" si="3"/>
-        <v>0.67941176470588238</v>
+        <v>0.85411764705882365</v>
       </c>
       <c r="H14" s="12">
         <v>0</v>
       </c>
       <c r="I14" s="15">
         <f t="shared" si="4"/>
-        <v>-0.2161764705882353</v>
+        <v>-0.34941176470588242</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="14">
         <f t="shared" si="5"/>
-        <v>0.46323529411764708</v>
+        <v>0.50470588235294123</v>
       </c>
       <c r="L14" s="14">
         <f t="shared" si="6"/>
-        <v>0.89558823529411768</v>
+        <v>1.203529411764706</v>
       </c>
       <c r="M14" s="6"/>
     </row>
@@ -1537,40 +1406,40 @@
       </c>
       <c r="B15" s="14">
         <f>'Target Allocation'!B14</f>
-        <v>0.60588235294117643</v>
+        <v>0.75882352941176467</v>
       </c>
       <c r="C15" s="15">
         <f t="shared" si="0"/>
-        <v>0.45441176470588229</v>
+        <v>0.49323529411764705</v>
       </c>
       <c r="D15" s="15">
         <f t="shared" si="1"/>
-        <v>0.66647058823529415</v>
+        <v>0.83470588235294119</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="14">
         <f t="shared" si="2"/>
-        <v>0.45441176470588229</v>
+        <v>0.49323529411764705</v>
       </c>
       <c r="G15" s="14">
         <f t="shared" si="3"/>
-        <v>0.66647058823529415</v>
+        <v>0.83470588235294119</v>
       </c>
       <c r="H15" s="12">
         <v>0</v>
       </c>
       <c r="I15" s="15">
         <f t="shared" si="4"/>
-        <v>-0.21205882352941186</v>
+        <v>-0.34147058823529414</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="14">
         <f t="shared" si="5"/>
-        <v>0.45441176470588229</v>
+        <v>0.49323529411764705</v>
       </c>
       <c r="L15" s="14">
         <f t="shared" si="6"/>
-        <v>0.878529411764706</v>
+        <v>1.1761764705882354</v>
       </c>
       <c r="M15" s="6"/>
     </row>
@@ -1581,40 +1450,40 @@
       </c>
       <c r="B16" s="14">
         <f>'Target Allocation'!B15</f>
-        <v>0.59411764705882353</v>
+        <v>0.74117647058823533</v>
       </c>
       <c r="C16" s="15">
         <f t="shared" si="0"/>
-        <v>0.44558823529411762</v>
+        <v>0.48176470588235298</v>
       </c>
       <c r="D16" s="15">
         <f t="shared" si="1"/>
-        <v>0.65352941176470591</v>
+        <v>0.81529411764705895</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="14">
         <f t="shared" si="2"/>
-        <v>0.44558823529411762</v>
+        <v>0.48176470588235298</v>
       </c>
       <c r="G16" s="14">
         <f t="shared" si="3"/>
-        <v>0.65352941176470591</v>
+        <v>0.81529411764705895</v>
       </c>
       <c r="H16" s="12">
         <v>0</v>
       </c>
       <c r="I16" s="15">
         <f t="shared" si="4"/>
-        <v>-0.2079411764705883</v>
+        <v>-0.33352941176470596</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="14">
         <f t="shared" si="5"/>
-        <v>0.44558823529411762</v>
+        <v>0.48176470588235298</v>
       </c>
       <c r="L16" s="14">
         <f t="shared" si="6"/>
-        <v>0.86147058823529421</v>
+        <v>1.1488235294117648</v>
       </c>
       <c r="M16" s="6"/>
     </row>
@@ -1625,40 +1494,40 @@
       </c>
       <c r="B17" s="14">
         <f>'Target Allocation'!B16</f>
-        <v>0.58235294117647052</v>
+        <v>0.72352941176470587</v>
       </c>
       <c r="C17" s="15">
         <f t="shared" si="0"/>
-        <v>0.43676470588235289</v>
+        <v>0.47029411764705881</v>
       </c>
       <c r="D17" s="15">
         <f t="shared" si="1"/>
-        <v>0.64058823529411757</v>
+        <v>0.79588235294117649</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="14">
         <f t="shared" si="2"/>
-        <v>0.43676470588235289</v>
+        <v>0.47029411764705881</v>
       </c>
       <c r="G17" s="14">
         <f t="shared" si="3"/>
-        <v>0.64058823529411757</v>
+        <v>0.79588235294117649</v>
       </c>
       <c r="H17" s="12">
         <v>0</v>
       </c>
       <c r="I17" s="15">
         <f t="shared" si="4"/>
-        <v>-0.20382352941176468</v>
+        <v>-0.32558823529411768</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="14">
         <f t="shared" si="5"/>
-        <v>0.43676470588235289</v>
+        <v>0.47029411764705881</v>
       </c>
       <c r="L17" s="14">
         <f t="shared" si="6"/>
-        <v>0.8444117647058822</v>
+        <v>1.1214705882352942</v>
       </c>
       <c r="M17" s="6"/>
     </row>
@@ -1669,40 +1538,40 @@
       </c>
       <c r="B18" s="14">
         <f>'Target Allocation'!B17</f>
-        <v>0.57058823529411762</v>
+        <v>0.70588235294117641</v>
       </c>
       <c r="C18" s="15">
         <f t="shared" si="0"/>
-        <v>0.42794117647058821</v>
+        <v>0.45882352941176469</v>
       </c>
       <c r="D18" s="15">
         <f t="shared" si="1"/>
-        <v>0.62764705882352945</v>
+        <v>0.77647058823529413</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="14">
         <f t="shared" si="2"/>
-        <v>0.42794117647058821</v>
+        <v>0.45882352941176469</v>
       </c>
       <c r="G18" s="14">
         <f t="shared" si="3"/>
-        <v>0.62764705882352945</v>
+        <v>0.77647058823529413</v>
       </c>
       <c r="H18" s="12">
         <v>0</v>
       </c>
       <c r="I18" s="15">
         <f t="shared" si="4"/>
-        <v>-0.19970588235294123</v>
+        <v>-0.31764705882352945</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="14">
         <f t="shared" si="5"/>
-        <v>0.42794117647058821</v>
+        <v>0.45882352941176469</v>
       </c>
       <c r="L18" s="14">
         <f t="shared" si="6"/>
-        <v>0.82735294117647062</v>
+        <v>1.0941176470588236</v>
       </c>
       <c r="M18" s="6"/>
     </row>
@@ -1713,40 +1582,40 @@
       </c>
       <c r="B19" s="14">
         <f>'Target Allocation'!B18</f>
-        <v>0.55882352941176472</v>
+        <v>0.68823529411764706</v>
       </c>
       <c r="C19" s="15">
         <f t="shared" si="0"/>
-        <v>0.41911764705882354</v>
+        <v>0.44735294117647062</v>
       </c>
       <c r="D19" s="15">
         <f t="shared" si="1"/>
-        <v>0.61470588235294121</v>
+        <v>0.75705882352941178</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="14">
         <f t="shared" si="2"/>
-        <v>0.41911764705882354</v>
+        <v>0.44735294117647062</v>
       </c>
       <c r="G19" s="14">
         <f t="shared" si="3"/>
-        <v>0.61470588235294121</v>
+        <v>0.75705882352941178</v>
       </c>
       <c r="H19" s="12">
         <v>0</v>
       </c>
       <c r="I19" s="15">
         <f t="shared" si="4"/>
-        <v>-0.19558823529411767</v>
+        <v>-0.30970588235294116</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="14">
         <f t="shared" si="5"/>
-        <v>0.41911764705882354</v>
+        <v>0.44735294117647062</v>
       </c>
       <c r="L19" s="14">
         <f t="shared" si="6"/>
-        <v>0.81029411764705883</v>
+        <v>1.0667647058823531</v>
       </c>
       <c r="M19" s="6"/>
     </row>
@@ -1757,40 +1626,40 @@
       </c>
       <c r="B20" s="14">
         <f>'Target Allocation'!B19</f>
-        <v>0.54705882352941171</v>
+        <v>0.6705882352941176</v>
       </c>
       <c r="C20" s="15">
         <f t="shared" si="0"/>
-        <v>0.41029411764705881</v>
+        <v>0.43588235294117644</v>
       </c>
       <c r="D20" s="15">
         <f t="shared" si="1"/>
-        <v>0.60176470588235298</v>
+        <v>0.73764705882352943</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="14">
         <f t="shared" si="2"/>
-        <v>0.41029411764705881</v>
+        <v>0.43588235294117644</v>
       </c>
       <c r="G20" s="14">
         <f t="shared" si="3"/>
-        <v>0.60176470588235298</v>
+        <v>0.73764705882352943</v>
       </c>
       <c r="H20" s="12">
         <v>0</v>
       </c>
       <c r="I20" s="15">
         <f t="shared" si="4"/>
-        <v>-0.19147058823529417</v>
+        <v>-0.30176470588235299</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="14">
         <f t="shared" si="5"/>
-        <v>0.41029411764705881</v>
+        <v>0.43588235294117644</v>
       </c>
       <c r="L20" s="14">
         <f t="shared" si="6"/>
-        <v>0.79323529411764715</v>
+        <v>1.0394117647058825</v>
       </c>
       <c r="M20" s="6"/>
     </row>
@@ -1801,40 +1670,40 @@
       </c>
       <c r="B21" s="14">
         <f>'Target Allocation'!B20</f>
-        <v>0.53529411764705881</v>
+        <v>0.65294117647058825</v>
       </c>
       <c r="C21" s="15">
         <f t="shared" si="0"/>
-        <v>0.40147058823529413</v>
+        <v>0.42441176470588238</v>
       </c>
       <c r="D21" s="15">
         <f t="shared" si="1"/>
-        <v>0.58882352941176475</v>
+        <v>0.71823529411764708</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="14">
         <f t="shared" si="2"/>
-        <v>0.40147058823529413</v>
+        <v>0.42441176470588238</v>
       </c>
       <c r="G21" s="14">
         <f t="shared" si="3"/>
-        <v>0.58882352941176475</v>
+        <v>0.71823529411764708</v>
       </c>
       <c r="H21" s="12">
         <v>0</v>
       </c>
       <c r="I21" s="15">
         <f t="shared" si="4"/>
-        <v>-0.18735294117647061</v>
+        <v>-0.29382352941176471</v>
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="14">
         <f t="shared" si="5"/>
-        <v>0.40147058823529413</v>
+        <v>0.42441176470588238</v>
       </c>
       <c r="L21" s="14">
         <f t="shared" si="6"/>
-        <v>0.77617647058823536</v>
+        <v>1.0120588235294119</v>
       </c>
       <c r="M21" s="6"/>
     </row>
@@ -1845,40 +1714,40 @@
       </c>
       <c r="B22" s="14">
         <f>'Target Allocation'!B21</f>
-        <v>0.5235294117647058</v>
+        <v>0.63529411764705879</v>
       </c>
       <c r="C22" s="15">
         <f t="shared" si="0"/>
-        <v>0.39264705882352935</v>
+        <v>0.4129411764705882</v>
       </c>
       <c r="D22" s="15">
         <f t="shared" si="1"/>
-        <v>0.5758823529411764</v>
+        <v>0.69882352941176473</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="14">
         <f t="shared" si="2"/>
-        <v>0.39264705882352935</v>
+        <v>0.4129411764705882</v>
       </c>
       <c r="G22" s="14">
         <f t="shared" si="3"/>
-        <v>0.5758823529411764</v>
+        <v>0.69882352941176473</v>
       </c>
       <c r="H22" s="12">
         <v>0</v>
       </c>
       <c r="I22" s="15">
         <f t="shared" si="4"/>
-        <v>-0.18323529411764705</v>
+        <v>-0.28588235294117653</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="14">
         <f t="shared" si="5"/>
-        <v>0.39264705882352935</v>
+        <v>0.4129411764705882</v>
       </c>
       <c r="L22" s="14">
         <f t="shared" si="6"/>
-        <v>0.75911764705882345</v>
+        <v>0.98470588235294132</v>
       </c>
       <c r="M22" s="6"/>
     </row>
@@ -1889,40 +1758,40 @@
       </c>
       <c r="B23" s="14">
         <f>'Target Allocation'!B22</f>
-        <v>0.5117647058823529</v>
+        <v>0.61764705882352944</v>
       </c>
       <c r="C23" s="15">
         <f t="shared" si="0"/>
-        <v>0.38382352941176467</v>
+        <v>0.40147058823529413</v>
       </c>
       <c r="D23" s="15">
         <f t="shared" si="1"/>
-        <v>0.56294117647058828</v>
+        <v>0.67941176470588238</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="14">
         <f t="shared" si="2"/>
-        <v>0.38382352941176467</v>
+        <v>0.40147058823529413</v>
       </c>
       <c r="G23" s="14">
         <f t="shared" si="3"/>
-        <v>0.56294117647058828</v>
+        <v>0.67941176470588238</v>
       </c>
       <c r="H23" s="12">
         <v>0</v>
       </c>
       <c r="I23" s="15">
         <f t="shared" si="4"/>
-        <v>-0.1791176470588236</v>
+        <v>-0.27794117647058825</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="14">
         <f t="shared" si="5"/>
-        <v>0.38382352941176467</v>
+        <v>0.40147058823529413</v>
       </c>
       <c r="L23" s="14">
         <f t="shared" si="6"/>
-        <v>0.74205882352941188</v>
+        <v>0.95735294117647063</v>
       </c>
       <c r="M23" s="6"/>
     </row>
@@ -1933,40 +1802,40 @@
       </c>
       <c r="B24" s="26">
         <f>'Target Allocation'!B23</f>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="C24" s="27">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.39</v>
       </c>
       <c r="D24" s="27">
         <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="26">
         <f t="shared" si="2"/>
-        <v>0.375</v>
+        <v>0.39</v>
       </c>
       <c r="G24" s="26">
         <f t="shared" si="3"/>
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H24" s="16">
         <v>0</v>
       </c>
       <c r="I24" s="27">
         <f t="shared" si="4"/>
-        <v>-0.17500000000000004</v>
+        <v>-0.27</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="26">
         <f t="shared" si="5"/>
-        <v>0.375</v>
+        <v>0.39</v>
       </c>
       <c r="L24" s="26">
         <f t="shared" si="6"/>
-        <v>0.72500000000000009</v>
+        <v>0.93</v>
       </c>
       <c r="M24" s="16"/>
     </row>
@@ -2001,7 +1870,7 @@
   <sheetPr>
     <tabColor theme="8" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2015,7 +1884,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -2023,815 +1892,379 @@
       <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="20">
-        <v>1.2</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <f>'Target Allocation'!A6</f>
-        <v>44561</v>
-      </c>
-      <c r="B7" s="14">
-        <f>'Target Allocation'!C6</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="15">
-        <f>B7*$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="15">
-        <f>B7*$B$3</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <f>'Target Allocation'!A7</f>
-        <v>44926</v>
-      </c>
-      <c r="B8" s="14">
-        <f>'Target Allocation'!C7</f>
-        <v>1.7647058823529412E-2</v>
-      </c>
-      <c r="C8" s="15">
-        <f t="shared" ref="C8:C24" si="0">B8*$B$2</f>
-        <v>8.8235294117647058E-3</v>
-      </c>
-      <c r="D8" s="15">
-        <f t="shared" ref="D8:D24" si="1">B8*$B$3</f>
-        <v>2.1176470588235293E-2</v>
-      </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <f>'Target Allocation'!A8</f>
-        <v>45291</v>
-      </c>
-      <c r="B9" s="14">
-        <f>'Target Allocation'!C8</f>
-        <v>3.5294117647058823E-2</v>
-      </c>
-      <c r="C9" s="15">
-        <f t="shared" si="0"/>
-        <v>1.7647058823529412E-2</v>
-      </c>
-      <c r="D9" s="15">
-        <f t="shared" si="1"/>
-        <v>4.2352941176470586E-2</v>
-      </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <f>'Target Allocation'!A9</f>
-        <v>45657</v>
-      </c>
-      <c r="B10" s="14">
-        <f>'Target Allocation'!C9</f>
-        <v>5.2941176470588235E-2</v>
-      </c>
-      <c r="C10" s="15">
-        <f t="shared" si="0"/>
-        <v>2.6470588235294117E-2</v>
-      </c>
-      <c r="D10" s="15">
-        <f t="shared" si="1"/>
-        <v>6.3529411764705876E-2</v>
-      </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
-        <f>'Target Allocation'!A10</f>
-        <v>46022</v>
-      </c>
-      <c r="B11" s="14">
-        <f>'Target Allocation'!C10</f>
-        <v>7.0588235294117646E-2</v>
-      </c>
-      <c r="C11" s="15">
-        <f t="shared" si="0"/>
-        <v>3.5294117647058823E-2</v>
-      </c>
-      <c r="D11" s="15">
-        <f t="shared" si="1"/>
-        <v>8.4705882352941173E-2</v>
-      </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
-        <f>'Target Allocation'!A11</f>
-        <v>46387</v>
-      </c>
-      <c r="B12" s="14">
-        <f>'Target Allocation'!C11</f>
-        <v>8.8235294117647051E-2</v>
-      </c>
-      <c r="C12" s="15">
-        <f t="shared" si="0"/>
-        <v>4.4117647058823525E-2</v>
-      </c>
-      <c r="D12" s="15">
-        <f t="shared" si="1"/>
-        <v>0.10588235294117646</v>
-      </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
-        <f>'Target Allocation'!A12</f>
-        <v>46752</v>
-      </c>
-      <c r="B13" s="14">
-        <f>'Target Allocation'!C12</f>
-        <v>0.10588235294117647</v>
-      </c>
-      <c r="C13" s="15">
-        <f t="shared" si="0"/>
-        <v>5.2941176470588235E-2</v>
-      </c>
-      <c r="D13" s="15">
-        <f t="shared" si="1"/>
-        <v>0.12705882352941175</v>
-      </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
-        <f>'Target Allocation'!A13</f>
-        <v>47118</v>
-      </c>
-      <c r="B14" s="14">
-        <f>'Target Allocation'!C13</f>
-        <v>0.12352941176470589</v>
-      </c>
-      <c r="C14" s="15">
-        <f t="shared" si="0"/>
-        <v>6.1764705882352944E-2</v>
-      </c>
-      <c r="D14" s="15">
-        <f t="shared" si="1"/>
-        <v>0.14823529411764705</v>
-      </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
-        <f>'Target Allocation'!A14</f>
-        <v>47483</v>
-      </c>
-      <c r="B15" s="14">
-        <f>'Target Allocation'!C14</f>
-        <v>0.14117647058823529</v>
-      </c>
-      <c r="C15" s="15">
-        <f t="shared" si="0"/>
-        <v>7.0588235294117646E-2</v>
-      </c>
-      <c r="D15" s="15">
-        <f t="shared" si="1"/>
-        <v>0.16941176470588235</v>
-      </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
-        <f>'Target Allocation'!A15</f>
-        <v>47848</v>
-      </c>
-      <c r="B16" s="14">
-        <f>'Target Allocation'!C15</f>
-        <v>0.1588235294117647</v>
-      </c>
-      <c r="C16" s="15">
-        <f t="shared" si="0"/>
-        <v>7.9411764705882348E-2</v>
-      </c>
-      <c r="D16" s="15">
-        <f t="shared" si="1"/>
-        <v>0.19058823529411764</v>
-      </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
-        <f>'Target Allocation'!A16</f>
-        <v>48213</v>
-      </c>
-      <c r="B17" s="14">
-        <f>'Target Allocation'!C16</f>
-        <v>0.1764705882352941</v>
-      </c>
-      <c r="C17" s="15">
-        <f t="shared" si="0"/>
-        <v>8.8235294117647051E-2</v>
-      </c>
-      <c r="D17" s="15">
-        <f t="shared" si="1"/>
-        <v>0.21176470588235291</v>
-      </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
-        <f>'Target Allocation'!A17</f>
-        <v>48579</v>
-      </c>
-      <c r="B18" s="14">
-        <f>'Target Allocation'!C17</f>
-        <v>0.19411764705882353</v>
-      </c>
-      <c r="C18" s="15">
-        <f t="shared" si="0"/>
-        <v>9.7058823529411767E-2</v>
-      </c>
-      <c r="D18" s="15">
-        <f t="shared" si="1"/>
-        <v>0.23294117647058823</v>
-      </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
-        <f>'Target Allocation'!A18</f>
-        <v>48944</v>
-      </c>
-      <c r="B19" s="14">
-        <f>'Target Allocation'!C18</f>
-        <v>0.21176470588235294</v>
-      </c>
-      <c r="C19" s="15">
-        <f t="shared" si="0"/>
-        <v>0.10588235294117647</v>
-      </c>
-      <c r="D19" s="15">
-        <f t="shared" si="1"/>
-        <v>0.2541176470588235</v>
-      </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
-        <f>'Target Allocation'!A19</f>
-        <v>49309</v>
-      </c>
-      <c r="B20" s="14">
-        <f>'Target Allocation'!C19</f>
-        <v>0.22941176470588234</v>
-      </c>
-      <c r="C20" s="15">
-        <f t="shared" si="0"/>
-        <v>0.11470588235294117</v>
-      </c>
-      <c r="D20" s="15">
-        <f t="shared" si="1"/>
-        <v>0.2752941176470588</v>
-      </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
-        <f>'Target Allocation'!A20</f>
-        <v>49674</v>
-      </c>
-      <c r="B21" s="14">
-        <f>'Target Allocation'!C20</f>
-        <v>0.24705882352941178</v>
-      </c>
-      <c r="C21" s="15">
-        <f t="shared" si="0"/>
-        <v>0.12352941176470589</v>
-      </c>
-      <c r="D21" s="15">
-        <f t="shared" si="1"/>
-        <v>0.2964705882352941</v>
-      </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
-        <f>'Target Allocation'!A21</f>
-        <v>50040</v>
-      </c>
-      <c r="B22" s="14">
-        <f>'Target Allocation'!C21</f>
-        <v>0.26470588235294118</v>
-      </c>
-      <c r="C22" s="15">
-        <f t="shared" si="0"/>
-        <v>0.13235294117647059</v>
-      </c>
-      <c r="D22" s="15">
-        <f t="shared" si="1"/>
-        <v>0.31764705882352939</v>
-      </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
-        <f>'Target Allocation'!A22</f>
-        <v>50405</v>
-      </c>
-      <c r="B23" s="14">
-        <f>'Target Allocation'!C22</f>
-        <v>0.28235294117647058</v>
-      </c>
-      <c r="C23" s="15">
-        <f t="shared" si="0"/>
-        <v>0.14117647058823529</v>
-      </c>
-      <c r="D23" s="15">
-        <f t="shared" si="1"/>
-        <v>0.33882352941176469</v>
-      </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="25">
-        <f>'Target Allocation'!A23</f>
-        <v>50770</v>
-      </c>
-      <c r="B24" s="27">
-        <f>'Target Allocation'!C23</f>
-        <v>0.3</v>
-      </c>
-      <c r="C24" s="27">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="D24" s="27">
-        <f t="shared" si="1"/>
-        <v>0.36</v>
-      </c>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:D5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5393E5A7-6842-4A99-B8FE-EF753AB15DA7}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:E23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="36" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="29" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <f>'Target Allocation'!A6</f>
         <v>44561</v>
       </c>
       <c r="B5" s="14">
-        <f>'Target Allocation'!D6</f>
-        <v>0.3</v>
+        <f>'Target Allocation'!C6</f>
+        <v>0.1</v>
       </c>
       <c r="C5" s="15">
-        <f>1-SUM('Global Equities'!D7,'Global FI and Alts ex. Reserve'!D7)</f>
-        <v>0.22999999999999998</v>
+        <f>1-'Global Equities'!D7</f>
+        <v>9.9999999999998979E-3</v>
       </c>
       <c r="D5" s="15">
-        <f>1-SUM('Global Equities'!C7,'Global FI and Alts ex. Reserve'!C7)</f>
-        <v>0.47500000000000009</v>
+        <f>1-'Global Equities'!C7</f>
+        <v>0.41499999999999992</v>
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <f>'Target Allocation'!A7</f>
         <v>44926</v>
       </c>
       <c r="B6" s="14">
-        <f>'Target Allocation'!D7</f>
-        <v>0.29411764705882354</v>
+        <f>'Target Allocation'!C7</f>
+        <v>0.11764705882352942</v>
       </c>
       <c r="C6" s="15">
-        <f>1-SUM('Global Equities'!D8,'Global FI and Alts ex. Reserve'!D8)</f>
-        <v>0.22176470588235297</v>
+        <f>1-'Global Equities'!D8</f>
+        <v>2.9411764705882248E-2</v>
       </c>
       <c r="D6" s="15">
-        <f>1-SUM('Global Equities'!C8,'Global FI and Alts ex. Reserve'!C8)</f>
-        <v>0.47500000000000009</v>
+        <f>1-'Global Equities'!C8</f>
+        <v>0.42647058823529416</v>
       </c>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <f>'Target Allocation'!A8</f>
         <v>45291</v>
       </c>
       <c r="B7" s="14">
-        <f>'Target Allocation'!D8</f>
-        <v>0.28823529411764703</v>
+        <f>'Target Allocation'!C8</f>
+        <v>0.13529411764705884</v>
       </c>
       <c r="C7" s="15">
-        <f>1-SUM('Global Equities'!D9,'Global FI and Alts ex. Reserve'!D9)</f>
-        <v>0.21352941176470586</v>
+        <f>1-'Global Equities'!D9</f>
+        <v>4.8823529411764599E-2</v>
       </c>
       <c r="D7" s="15">
-        <f>1-SUM('Global Equities'!C9,'Global FI and Alts ex. Reserve'!C9)</f>
-        <v>0.47499999999999998</v>
+        <f>1-'Global Equities'!C9</f>
+        <v>0.43794117647058817</v>
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <f>'Target Allocation'!A9</f>
         <v>45657</v>
       </c>
       <c r="B8" s="14">
-        <f>'Target Allocation'!D9</f>
-        <v>0.28235294117647058</v>
+        <f>'Target Allocation'!C9</f>
+        <v>0.15294117647058825</v>
       </c>
       <c r="C8" s="15">
-        <f>1-SUM('Global Equities'!D10,'Global FI and Alts ex. Reserve'!D10)</f>
-        <v>0.20529411764705885</v>
+        <f>1-'Global Equities'!D10</f>
+        <v>6.823529411764695E-2</v>
       </c>
       <c r="D8" s="15">
-        <f>1-SUM('Global Equities'!C10,'Global FI and Alts ex. Reserve'!C10)</f>
-        <v>0.47499999999999998</v>
+        <f>1-'Global Equities'!C10</f>
+        <v>0.44941176470588229</v>
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <f>'Target Allocation'!A10</f>
         <v>46022</v>
       </c>
       <c r="B9" s="14">
-        <f>'Target Allocation'!D10</f>
-        <v>0.27647058823529413</v>
+        <f>'Target Allocation'!C10</f>
+        <v>0.17058823529411765</v>
       </c>
       <c r="C9" s="15">
-        <f>1-SUM('Global Equities'!D11,'Global FI and Alts ex. Reserve'!D11)</f>
-        <v>0.19705882352941173</v>
+        <f>1-'Global Equities'!D11</f>
+        <v>8.76470588235293E-2</v>
       </c>
       <c r="D9" s="15">
-        <f>1-SUM('Global Equities'!C11,'Global FI and Alts ex. Reserve'!C11)</f>
-        <v>0.47499999999999998</v>
+        <f>1-'Global Equities'!C11</f>
+        <v>0.46088235294117641</v>
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <f>'Target Allocation'!A11</f>
         <v>46387</v>
       </c>
       <c r="B10" s="14">
-        <f>'Target Allocation'!D11</f>
-        <v>0.27058823529411763</v>
+        <f>'Target Allocation'!C11</f>
+        <v>0.18823529411764708</v>
       </c>
       <c r="C10" s="15">
-        <f>1-SUM('Global Equities'!D12,'Global FI and Alts ex. Reserve'!D12)</f>
-        <v>0.18882352941176472</v>
+        <f>1-'Global Equities'!D12</f>
+        <v>0.10705882352941165</v>
       </c>
       <c r="D10" s="15">
-        <f>1-SUM('Global Equities'!C12,'Global FI and Alts ex. Reserve'!C12)</f>
-        <v>0.47500000000000009</v>
+        <f>1-'Global Equities'!C12</f>
+        <v>0.47235294117647053</v>
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <f>'Target Allocation'!A12</f>
         <v>46752</v>
       </c>
       <c r="B11" s="14">
-        <f>'Target Allocation'!D12</f>
-        <v>0.26470588235294118</v>
+        <f>'Target Allocation'!C12</f>
+        <v>0.20588235294117649</v>
       </c>
       <c r="C11" s="15">
-        <f>1-SUM('Global Equities'!D13,'Global FI and Alts ex. Reserve'!D13)</f>
-        <v>0.18058823529411761</v>
+        <f>1-'Global Equities'!D13</f>
+        <v>0.126470588235294</v>
       </c>
       <c r="D11" s="15">
-        <f>1-SUM('Global Equities'!C13,'Global FI and Alts ex. Reserve'!C13)</f>
-        <v>0.47499999999999998</v>
+        <f>1-'Global Equities'!C13</f>
+        <v>0.48382352941176465</v>
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <f>'Target Allocation'!A13</f>
         <v>47118</v>
       </c>
       <c r="B12" s="14">
-        <f>'Target Allocation'!D13</f>
-        <v>0.25882352941176467</v>
+        <f>'Target Allocation'!C13</f>
+        <v>0.22352941176470592</v>
       </c>
       <c r="C12" s="15">
-        <f>1-SUM('Global Equities'!D14,'Global FI and Alts ex. Reserve'!D14)</f>
-        <v>0.1723529411764706</v>
+        <f>1-'Global Equities'!D14</f>
+        <v>0.14588235294117635</v>
       </c>
       <c r="D12" s="15">
-        <f>1-SUM('Global Equities'!C14,'Global FI and Alts ex. Reserve'!C14)</f>
-        <v>0.47499999999999998</v>
+        <f>1-'Global Equities'!C14</f>
+        <v>0.49529411764705877</v>
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <f>'Target Allocation'!A14</f>
         <v>47483</v>
       </c>
       <c r="B13" s="14">
-        <f>'Target Allocation'!D14</f>
-        <v>0.25294117647058822</v>
+        <f>'Target Allocation'!C14</f>
+        <v>0.24117647058823533</v>
       </c>
       <c r="C13" s="15">
-        <f>1-SUM('Global Equities'!D15,'Global FI and Alts ex. Reserve'!D15)</f>
-        <v>0.16411764705882348</v>
+        <f>1-'Global Equities'!D15</f>
+        <v>0.16529411764705881</v>
       </c>
       <c r="D13" s="15">
-        <f>1-SUM('Global Equities'!C15,'Global FI and Alts ex. Reserve'!C15)</f>
-        <v>0.47500000000000009</v>
+        <f>1-'Global Equities'!C15</f>
+        <v>0.50676470588235301</v>
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <f>'Target Allocation'!A15</f>
         <v>47848</v>
       </c>
       <c r="B14" s="14">
-        <f>'Target Allocation'!D15</f>
-        <v>0.24705882352941178</v>
+        <f>'Target Allocation'!C15</f>
+        <v>0.25882352941176473</v>
       </c>
       <c r="C14" s="15">
-        <f>1-SUM('Global Equities'!D16,'Global FI and Alts ex. Reserve'!D16)</f>
-        <v>0.15588235294117647</v>
+        <f>1-'Global Equities'!D16</f>
+        <v>0.18470588235294105</v>
       </c>
       <c r="D14" s="15">
-        <f>1-SUM('Global Equities'!C16,'Global FI and Alts ex. Reserve'!C16)</f>
-        <v>0.47500000000000009</v>
+        <f>1-'Global Equities'!C16</f>
+        <v>0.51823529411764702</v>
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <f>'Target Allocation'!A16</f>
         <v>48213</v>
       </c>
       <c r="B15" s="14">
-        <f>'Target Allocation'!D16</f>
-        <v>0.2411764705882353</v>
+        <f>'Target Allocation'!C16</f>
+        <v>0.27647058823529413</v>
       </c>
       <c r="C15" s="15">
-        <f>1-SUM('Global Equities'!D17,'Global FI and Alts ex. Reserve'!D17)</f>
-        <v>0.14764705882352946</v>
+        <f>1-'Global Equities'!D17</f>
+        <v>0.20411764705882351</v>
       </c>
       <c r="D15" s="15">
-        <f>1-SUM('Global Equities'!C17,'Global FI and Alts ex. Reserve'!C17)</f>
-        <v>0.47500000000000009</v>
+        <f>1-'Global Equities'!C17</f>
+        <v>0.52970588235294125</v>
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <f>'Target Allocation'!A17</f>
         <v>48579</v>
       </c>
       <c r="B16" s="14">
-        <f>'Target Allocation'!D17</f>
-        <v>0.23529411764705882</v>
+        <f>'Target Allocation'!C17</f>
+        <v>0.29411764705882359</v>
       </c>
       <c r="C16" s="15">
-        <f>1-SUM('Global Equities'!D18,'Global FI and Alts ex. Reserve'!D18)</f>
-        <v>0.13941176470588235</v>
+        <f>1-'Global Equities'!D18</f>
+        <v>0.22352941176470587</v>
       </c>
       <c r="D16" s="15">
-        <f>1-SUM('Global Equities'!C18,'Global FI and Alts ex. Reserve'!C18)</f>
-        <v>0.47499999999999998</v>
+        <f>1-'Global Equities'!C18</f>
+        <v>0.54117647058823537</v>
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <f>'Target Allocation'!A18</f>
         <v>48944</v>
       </c>
       <c r="B17" s="14">
-        <f>'Target Allocation'!D18</f>
-        <v>0.22941176470588237</v>
+        <f>'Target Allocation'!C18</f>
+        <v>0.31176470588235294</v>
       </c>
       <c r="C17" s="15">
-        <f>1-SUM('Global Equities'!D19,'Global FI and Alts ex. Reserve'!D19)</f>
-        <v>0.13117647058823523</v>
+        <f>1-'Global Equities'!D19</f>
+        <v>0.24294117647058822</v>
       </c>
       <c r="D17" s="15">
-        <f>1-SUM('Global Equities'!C19,'Global FI and Alts ex. Reserve'!C19)</f>
-        <v>0.47499999999999998</v>
+        <f>1-'Global Equities'!C19</f>
+        <v>0.55264705882352938</v>
       </c>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <f>'Target Allocation'!A19</f>
         <v>49309</v>
       </c>
       <c r="B18" s="14">
-        <f>'Target Allocation'!D19</f>
-        <v>0.22352941176470587</v>
+        <f>'Target Allocation'!C19</f>
+        <v>0.3294117647058824</v>
       </c>
       <c r="C18" s="15">
-        <f>1-SUM('Global Equities'!D20,'Global FI and Alts ex. Reserve'!D20)</f>
-        <v>0.12294117647058822</v>
+        <f>1-'Global Equities'!D20</f>
+        <v>0.26235294117647057</v>
       </c>
       <c r="D18" s="15">
-        <f>1-SUM('Global Equities'!C20,'Global FI and Alts ex. Reserve'!C20)</f>
-        <v>0.47499999999999998</v>
+        <f>1-'Global Equities'!C20</f>
+        <v>0.56411764705882361</v>
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <f>'Target Allocation'!A20</f>
         <v>49674</v>
       </c>
       <c r="B19" s="14">
-        <f>'Target Allocation'!D20</f>
-        <v>0.21764705882352942</v>
+        <f>'Target Allocation'!C20</f>
+        <v>0.34705882352941181</v>
       </c>
       <c r="C19" s="15">
-        <f>1-SUM('Global Equities'!D21,'Global FI and Alts ex. Reserve'!D21)</f>
-        <v>0.11470588235294121</v>
+        <f>1-'Global Equities'!D21</f>
+        <v>0.28176470588235292</v>
       </c>
       <c r="D19" s="15">
-        <f>1-SUM('Global Equities'!C21,'Global FI and Alts ex. Reserve'!C21)</f>
-        <v>0.47499999999999998</v>
+        <f>1-'Global Equities'!C21</f>
+        <v>0.57558823529411762</v>
       </c>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <f>'Target Allocation'!A21</f>
         <v>50040</v>
       </c>
       <c r="B20" s="14">
-        <f>'Target Allocation'!D21</f>
-        <v>0.21176470588235294</v>
+        <f>'Target Allocation'!C21</f>
+        <v>0.36470588235294121</v>
       </c>
       <c r="C20" s="15">
-        <f>1-SUM('Global Equities'!D22,'Global FI and Alts ex. Reserve'!D22)</f>
-        <v>0.10647058823529421</v>
+        <f>1-'Global Equities'!D22</f>
+        <v>0.30117647058823527</v>
       </c>
       <c r="D20" s="15">
-        <f>1-SUM('Global Equities'!C22,'Global FI and Alts ex. Reserve'!C22)</f>
-        <v>0.47500000000000009</v>
+        <f>1-'Global Equities'!C22</f>
+        <v>0.58705882352941186</v>
       </c>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <f>'Target Allocation'!A22</f>
         <v>50405</v>
       </c>
       <c r="B21" s="14">
-        <f>'Target Allocation'!D22</f>
-        <v>0.20588235294117646</v>
+        <f>'Target Allocation'!C22</f>
+        <v>0.38235294117647067</v>
       </c>
       <c r="C21" s="15">
-        <f>1-SUM('Global Equities'!D23,'Global FI and Alts ex. Reserve'!D23)</f>
-        <v>9.8235294117646976E-2</v>
+        <f>1-'Global Equities'!D23</f>
+        <v>0.32058823529411762</v>
       </c>
       <c r="D21" s="15">
-        <f>1-SUM('Global Equities'!C23,'Global FI and Alts ex. Reserve'!C23)</f>
-        <v>0.47500000000000009</v>
+        <f>1-'Global Equities'!C23</f>
+        <v>0.59852941176470587</v>
       </c>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <f>'Target Allocation'!A23</f>
         <v>50770</v>
       </c>
       <c r="B22" s="27">
-        <f>'Target Allocation'!D23</f>
-        <v>0.2</v>
+        <f>'Target Allocation'!C23</f>
+        <v>0.4</v>
       </c>
       <c r="C22" s="27">
-        <f>1-SUM('Global Equities'!D24,'Global FI and Alts ex. Reserve'!D24)</f>
-        <v>8.9999999999999969E-2</v>
+        <f>1-'Global Equities'!D24</f>
+        <v>0.33999999999999997</v>
       </c>
       <c r="D22" s="27">
-        <f>1-SUM('Global Equities'!C24,'Global FI and Alts ex. Reserve'!C24)</f>
-        <v>0.47499999999999998</v>
+        <f>1-'Global Equities'!C24</f>
+        <v>0.61</v>
       </c>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>

</xml_diff>